<commit_message>
004sp toco lgbm y variables para recortar
</commit_message>
<xml_diff>
--- a/src/workflow-semillerio/Experimentos.xlsx
+++ b/src/workflow-semillerio/Experimentos.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Documents\GitHub\labo2023r\src\workflow-semillerio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F1BB58-ED49-434D-8D97-F0F723FF9A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E60774B-05CB-40A2-B1CD-FFBFC3FEF720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="exp" sheetId="2" r:id="rId2"/>
+    <sheet name="rdos" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
   <si>
     <t>enriquevegasua@gmail.com</t>
   </si>
@@ -173,12 +174,124 @@
 PARAM$train$validation &lt;- c(202106)
 PARAM$train$testing &lt;- c(202107)</t>
   </si>
+  <si>
+    <t>ZZ7710_002sp_03_001_10500p</t>
+  </si>
+  <si>
+    <t>archivo</t>
+  </si>
+  <si>
+    <t>drive</t>
+  </si>
+  <si>
+    <t>infortunio</t>
+  </si>
+  <si>
+    <t>Gcia</t>
+  </si>
+  <si>
+    <t>ZZ7710_002sp_03_001_11000p</t>
+  </si>
+  <si>
+    <t>ZZ7710_002sp_03_001_11500p</t>
+  </si>
+  <si>
+    <t>ZZ7710_002sp_03_001_12000p</t>
+  </si>
+  <si>
+    <t>ZZ7710_002sp_03_001_12500p</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>enriquevegasua</t>
+  </si>
+  <si>
+    <t>vm004sp-lasvegas-ev</t>
+  </si>
+  <si>
+    <t>elimino variables mai, dejo las mias</t>
+  </si>
+  <si>
+    <t>PARAM$Tendencias1$run &lt;- TRUE
+PARAM$Tendencias1$ventana &lt;- 3
+PARAM$Tendencias1$tendencia &lt;- TRUE
+PARAM$Tendencias1$minimo &lt;- FALSE
+PARAM$Tendencias1$maximo &lt;- FALSE
+PARAM$Tendencias1$promedio &lt;- TRUE
+PARAM$Tendencias1$ratioavg &lt;- FALSE
+PARAM$Tendencias1$ratiomax &lt;- FALSE
+PARAM$Tendencias2$run &lt;- TRUE
+PARAM$Tendencias2$ventana &lt;- 6
+PARAM$Tendencias2$tendencia &lt;- TRUE
+PARAM$Tendencias2$minimo &lt;- FALSE
+PARAM$Tendencias2$maximo &lt;- FALSE
+PARAM$Tendencias2$promedio &lt;- TRUE
+PARAM$Tendencias2$ratioavg &lt;- FALSE
+PARAM$Tendencias2$ratiomax &lt;- FALSE
+PARAM$RandomForest$run &lt;- TRUE
+PARAM$RandomForest$num.trees &lt;- 300
+PARAM$RandomForest$max.depth &lt;- 8
+PARAM$RandomForest$min.node.size &lt;- 700
+PARAM$RandomForest$mtry &lt;- 75
+PARAM$RandomForest$semilla &lt;- 666667 # cambiar por la propia semilla
+# varia de 0.0 a 2.0, si es 0.0 NO se activan
+PARAM$CanaritosAsesinos$ratio &lt;- 0.66
+# desvios estandar de la media, para el cutoff
+PARAM$CanaritosAsesinos$desvios &lt;- 2</t>
+  </si>
+  <si>
+    <t>PARAM$train$undersampling &lt;- 0.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+# Hiperparametros FIJOS de  lightgbm
+PARAM$lgb_basicos &lt;- list(
+  boosting = "gbdt", # puede ir  dart  , ni pruebe random_forest
+  objective = "binary",
+  metric = "custom",
+  first_metric_only = TRUE,
+  boost_from_average = TRUE,
+  feature_pre_filter = FALSE,
+  force_row_wise = TRUE, # para reducir warnings
+  verbosity = -100,
+  max_depth = 8.0, #-1L, # -1 significa no limitar,  por ahora lo dejo fijo
+  min_gain_to_split = 3.0, # min_gain_to_split &gt;= 0.0
+  min_sum_hessian_in_leaf = 0.001, #  min_sum_hessian_in_leaf &gt;= 0.0
+  lambda_l1 = 0.1, # lambda_l1 &gt;= 0.0
+  lambda_l2 = 0.1, # lambda_l2 &gt;= 0.0
+  max_bin = 31L, # lo debo dejar fijo, no participa de la BO
+  num_iterations = 9999, # un numero muy grande, lo limita early_stopping_rounds
+  bagging_fraction = 0.6, # 0.0 &lt; bagging_fraction &lt;= 1.0
+  pos_bagging_fraction = 0.6, # 0.0 &lt; pos_bagging_fraction &lt;= 1.0
+  neg_bagging_fraction = 0.6, # 0.0 &lt; neg_bagging_fraction &lt;= 1.0
+  is_unbalance = FALSE, #
+  scale_pos_weight = 1.0, # scale_pos_weight &gt; 0.0
+  drop_rate = 0.1, # 0.0 &lt; neg_bagging_fraction &lt;= 1.0
+  max_drop = 50, # &lt;=0 means no limit
+  skip_drop = 0.5, # 0.0 &lt;= skip_drop &lt;= 1.0
+  extra_trees = TRUE, # Magic Sauce
+  seed = PARAM$lgb_semilla
+)</t>
+  </si>
+  <si>
+    <t>PARAM$semillerio &lt;- 25
+# se utiliza para generar el vector de  PARAM$semillerio  semillas
+PARAM$semilla_primos &lt;- 666707
+PARAM$kaggle$envios_desde &lt;- 10000L
+PARAM$kaggle$envios_hasta &lt;- 12000L
+PARAM$kaggle$envios_salto &lt;- 500L</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,16 +321,35 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -225,23 +357,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -621,140 +779,305 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96723825-D687-48AB-A668-4A5F8C2B6B23}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="40.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="66.28515625" customWidth="1"/>
-    <col min="13" max="13" width="100.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.5703125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="38.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.42578125" style="11"/>
+    <col min="12" max="12" width="66.28515625" style="11" customWidth="1"/>
+    <col min="13" max="14" width="100.28515625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="9">
         <v>771</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="9">
         <v>731</v>
       </c>
-      <c r="M1">
+      <c r="M1" s="9">
         <v>741</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="N1" s="9">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="11">
         <v>0.5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="11">
         <v>0.5</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="12">
         <v>69.739485000000002</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="11">
         <v>0.5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="11">
         <v>0.5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" s="12">
+        <f>rdos!E4</f>
+        <v>49.449102000000003</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="13">
         <v>20230717073300</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="11">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="11">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="14" t="s">
         <v>41</v>
+      </c>
+      <c r="N4" s="14"/>
+    </row>
+    <row r="5" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0.66</v>
+      </c>
+      <c r="D5" s="11">
+        <v>2</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25FCFFD-2E80-4959-9D99-0D58E79A0770}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="6">
+        <v>49.839089999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="6">
+        <v>49.139110000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="6">
+        <v>49.559100000000001</v>
+      </c>
+      <c r="E4" s="7">
+        <f>AVERAGE(D2:D6)</f>
+        <v>49.449102000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="6">
+        <v>49.539099999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="6">
+        <v>49.169110000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
004 light el anterior se suicido en FE
</commit_message>
<xml_diff>
--- a/src/workflow-semillerio/Experimentos.xlsx
+++ b/src/workflow-semillerio/Experimentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Documents\GitHub\labo2023r\src\workflow-semillerio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E60774B-05CB-40A2-B1CD-FFBFC3FEF720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93154DA7-6A81-4A88-B6CD-CB309BD69F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>enriquevegasua@gmail.com</t>
   </si>
@@ -282,6 +282,15 @@
 PARAM$kaggle$envios_desde &lt;- 10000L
 PARAM$kaggle$envios_hasta &lt;- 12000L
 PARAM$kaggle$envios_salto &lt;- 500L</t>
+  </si>
+  <si>
+    <t>004sp</t>
+  </si>
+  <si>
+    <t>20230717 224000</t>
+  </si>
+  <si>
+    <t>20230717 073300</t>
   </si>
 </sst>
 </file>
@@ -781,8 +790,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96723825-D687-48AB-A668-4A5F8C2B6B23}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,8 +900,8 @@
       <c r="H3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="13">
-        <v>20230717073300</v>
+      <c r="I3" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>36</v>
@@ -935,7 +945,7 @@
     </row>
     <row r="5" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>52</v>
@@ -954,6 +964,9 @@
       </c>
       <c r="H5" s="11" t="s">
         <v>53</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="K5" s="11" t="s">
         <v>54</v>

</xml_diff>